<commit_message>
add a function for notification
</commit_message>
<xml_diff>
--- a/public/reports/Marketplace_Report.xlsx
+++ b/public/reports/Marketplace_Report.xlsx
@@ -16,7 +16,7 @@
     <t>Generated on:</t>
   </si>
   <si>
-    <t>March 12, 2025 at 11:31:47 PM</t>
+    <t>March 22, 2025 at 03:34:21 PM</t>
   </si>
   <si>
     <t>Total Users:</t>
@@ -25,7 +25,7 @@
     <t>Total Sales (₱):</t>
   </si>
   <si>
-    <t>8,462</t>
+    <t>3,423</t>
   </si>
   <si>
     <t>Total Auction Sessions:</t>
@@ -498,7 +498,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -537,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -548,13 +548,13 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>8462</v>
+        <v>3423</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,13 +688,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="1">
-        <v>8462</v>
+        <v>3423</v>
       </c>
       <c r="C20" s="1">
         <v>6</v>
       </c>
       <c r="D20" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>